<commit_message>
Loss too large, paused at 13/30 epochs.
</commit_message>
<xml_diff>
--- a/training_log.xlsx
+++ b/training_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/50772f30bd668d95/Documents/NYCU/ML/hw4/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="82" documentId="11_AD4DBB64A54DDB1B405E38FC2D1807BF4E90DF24" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AEF389E6-5DC7-4E59-BFB3-03099A368DA8}"/>
+  <xr:revisionPtr revIDLastSave="83" documentId="11_AD4DBB64A54DDB1B405E38FC2D1807BF4E90DF24" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D25A4C85-AD49-41D3-8937-AD8C1FC38C73}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>new changes</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -93,6 +93,9 @@
   <si>
     <t>back to 1205_1636 setting</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>early stopping, a learning rate scheduler, regularization, stronger augmentation, and dropout</t>
   </si>
 </sst>
 </file>
@@ -424,10 +427,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -557,6 +560,11 @@
         <v>16</v>
       </c>
     </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K7" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
0.22985 at 19/30 epoch.
</commit_message>
<xml_diff>
--- a/training_log.xlsx
+++ b/training_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/50772f30bd668d95/Documents/NYCU/ML/hw4/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="83" documentId="11_AD4DBB64A54DDB1B405E38FC2D1807BF4E90DF24" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D25A4C85-AD49-41D3-8937-AD8C1FC38C73}"/>
+  <xr:revisionPtr revIDLastSave="88" documentId="11_AD4DBB64A54DDB1B405E38FC2D1807BF4E90DF24" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4FF8516A-F21B-4A5E-9075-FE1BEDA0FDA6}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>new changes</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -87,15 +87,20 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>early end at</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>back to 1205_1636 setting</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>early stopping, a learning rate scheduler, regularization, stronger augmentation, and dropout</t>
+    <t>early stop at</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>early stopping, warm up, slow down, random sample, random split</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>some trials, not successful</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -427,10 +432,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -471,7 +476,7 @@
         <v>3</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>0</v>
@@ -557,11 +562,16 @@
         <v>10</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K8" s="1" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>